<commit_message>
Update to vcc citibank pic data
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kalyana\Traveloka_DataAutomation_Performer_Gsheet\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kalyana\Gsheet Sprint 3\Traveloka_DataAutomation_Performer_Gsheet\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{487F17F2-49EB-4D4E-AAA9-E9B2CA9E73B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B80A36D2-BC93-4C39-8E12-EF41E2E7C18B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3384" yWindow="3384" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -177,15 +177,9 @@
     <t>GlobalVarAsset</t>
   </si>
   <si>
-    <t>EmailRawFolderName</t>
-  </si>
-  <si>
     <t>[Dev] RPA_Moon_UploadBucket</t>
   </si>
   <si>
-    <t>Email_Raw_Data</t>
-  </si>
-  <si>
     <t>[Dev] RPA_Moon_PathMailTemplate</t>
   </si>
   <si>
@@ -225,13 +219,19 @@
     <t>[Dev] RPA_Moon_Gsheet</t>
   </si>
   <si>
-    <t>RPA_Moon_Gsheet_Date</t>
-  </si>
-  <si>
     <t>PathSAKey</t>
   </si>
   <si>
     <t>[Dev] RPA_Moon_PathSaKey</t>
+  </si>
+  <si>
+    <t>Gsheet_Raw_Data</t>
+  </si>
+  <si>
+    <t>RawFolderName</t>
+  </si>
+  <si>
+    <t>[Dev] RPA_Moon_Gsheet_Date</t>
   </si>
 </sst>
 </file>
@@ -610,7 +610,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -660,7 +660,7 @@
         <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -692,7 +692,7 @@
         <v>47</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -700,7 +700,7 @@
         <v>48</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -708,15 +708,15 @@
         <v>49</v>
       </c>
       <c r="B8" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -2881,9 +2881,6 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <customProperties>
-    <customPr name="EpmWorksheetKeyString_GUID" r:id="rId1"/>
-  </customProperties>
 </worksheet>
 </file>
 
@@ -2892,7 +2889,7 @@
   <dimension ref="A1:Z995"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:B9"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -2944,7 +2941,7 @@
         <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
@@ -2957,50 +2954,50 @@
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>